<commit_message>
Added A .odsReader for windows
</commit_message>
<xml_diff>
--- a/BOP_output_urlsNEW.xlsx
+++ b/BOP_output_urlsNEW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Exlterra CAD 02\Documents\GitHub\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380E8C7C-31FF-4DAC-B834-A59B8ACDFD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C7037BB-CF3C-4208-AD7A-8056DE846343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="2">
+  <futureMetadata name="XLRICHVALUE" count="5">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -52,13 +52,43 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="3"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="4"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="2">
+  <valueMetadata count="5">
     <bk>
       <rc t="1" v="0"/>
     </bk>
     <bk>
       <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+    <bk>
+      <rc t="1" v="3"/>
+    </bk>
+    <bk>
+      <rc t="1" v="4"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -1411,11 +1441,23 @@
     <address r:id="rId3"/>
     <blip r:id="rId4"/>
   </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId5"/>
+    <blip r:id="rId6"/>
+  </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId7"/>
+    <blip r:id="rId8"/>
+  </webImageSrd>
+  <webImageSrd>
+    <address r:id="rId9"/>
+    <blip r:id="rId10"/>
+  </webImageSrd>
 </webImagesSrd>
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
   <rv s="0">
     <v>0</v>
     <v>1</v>
@@ -1424,6 +1466,24 @@
   </rv>
   <rv s="0">
     <v>1</v>
+    <v>1</v>
+    <v>0</v>
+    <v>0</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
+    <v>1</v>
+    <v>0</v>
+    <v>0</v>
+  </rv>
+  <rv s="0">
+    <v>3</v>
+    <v>1</v>
+    <v>0</v>
+    <v>0</v>
+  </rv>
+  <rv s="0">
+    <v>4</v>
     <v>1</v>
     <v>0</v>
     <v>0</v>
@@ -1729,8 +1789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,9 +1871,9 @@
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="1" t="e">
-        <f t="shared" ref="E2:E33" ca="1" si="0">_xludf.IMAGE(B5)</f>
-        <v>#NAME?</v>
+      <c r="E5" s="1" t="e" vm="3">
+        <f>_xlfn.IMAGE(B5)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="225" x14ac:dyDescent="0.25">
@@ -1826,9 +1886,9 @@
       <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="1" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+      <c r="E6" s="1" t="e" vm="4">
+        <f>_xlfn.IMAGE(B6)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="180" x14ac:dyDescent="0.25">
@@ -1841,9 +1901,9 @@
       <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="1" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+      <c r="E7" s="1" t="e" vm="5">
+        <f>_xlfn.IMAGE(B7)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="180" x14ac:dyDescent="0.25">
@@ -1857,7 +1917,7 @@
         <v>22</v>
       </c>
       <c r="E8" s="1" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="E5:E33" ca="1" si="0">_xludf.IMAGE(B8)</f>
         <v>#NAME?</v>
       </c>
     </row>

</xml_diff>